<commit_message>
Added code to get Export Excel in Results folder
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Leave_Scenarios.xlsx
+++ b/src/main/resources/TestData/Leave_Scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="All_Scenarios" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,6 +20,7 @@
     <sheet name="Old_Scenarios" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">All_Scenarios!$A$1:$U$247</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">All_Without_Probation!$A$1:$U$83</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -4822,6 +4823,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -4829,19 +4834,19 @@
   </sheetPr>
   <dimension ref="A1:U247"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A147" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B148" activeCellId="0" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.5"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20900,6 +20905,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U247"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -20907,6 +20913,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -20923,9 +20930,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25096,21 +25104,21 @@
   </sheetPr>
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="0" topLeftCell="D83" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
+      <selection pane="topRight" activeCell="C96" activeCellId="0" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.5"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30526,19 +30534,19 @@
   </sheetPr>
   <dimension ref="A1:U165"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A164" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E164" activeCellId="0" sqref="E164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.5"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41290,13 +41298,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.5"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46718,9 +46726,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52142,10 +52150,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57567,9 +57576,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.3265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62991,13 +62998,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.5"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76609,9 +76616,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Final FrameWork that can be committed to master
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Leave_Scenarios.xlsx
+++ b/src/main/resources/TestData/Leave_Scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="All_Scenarios" sheetId="1" state="visible" r:id="rId2"/>
@@ -5327,19 +5327,19 @@
   </sheetPr>
   <dimension ref="A1:U247"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A247" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C257" activeCellId="0" sqref="C257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21421,7 +21421,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21459,10 +21460,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25633,15 +25635,13 @@
   </sheetPr>
   <dimension ref="A1:U165"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36395,13 +36395,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41823,13 +41823,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52581,13 +52581,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -58003,15 +58003,15 @@
   </sheetPr>
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K83" activeCellId="0" sqref="K83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -63433,11 +63433,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -68859,7 +68857,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74281,13 +74281,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>